<commit_message>
finishing problem 6 in the cs-513 final
</commit_message>
<xml_diff>
--- a/CS-513/FinalExam/final_problem6.xlsx
+++ b/CS-513/FinalExam/final_problem6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyatthenryblair/Desktop/Projects/Stevens/CS-513/FinalExam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7469f130076e6149/Desktop/Projects/Stevens/CS-513/FinalExam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA290C60-1578-DD4B-93BA-BB6E6A1759B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{AA290C60-1578-DD4B-93BA-BB6E6A1759B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9791AD50-124E-4377-8076-D457965B2D78}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="800" windowWidth="28040" windowHeight="17440" xr2:uid="{5CD4EC78-82A5-1D4F-B2C7-988FE798375A}"/>
+    <workbookView xWindow="38295" yWindow="9390" windowWidth="14610" windowHeight="15585" xr2:uid="{5CD4EC78-82A5-1D4F-B2C7-988FE798375A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
   <si>
     <t>From</t>
   </si>
@@ -267,14 +267,87 @@
   <si>
     <t>dE / dw_4-&gt;B</t>
   </si>
+  <si>
+    <t>net_A</t>
+  </si>
+  <si>
+    <t>net_B</t>
+  </si>
+  <si>
+    <t>out_A</t>
+  </si>
+  <si>
+    <t>out_B</t>
+  </si>
+  <si>
+    <t>net_z</t>
+  </si>
+  <si>
+    <t>out_z</t>
+  </si>
+  <si>
+    <t>learning_rate</t>
+  </si>
+  <si>
+    <t>new w_xx-&gt;z</t>
+  </si>
+  <si>
+    <t>new w_A-&gt;z</t>
+  </si>
+  <si>
+    <t>new w_B-&gt;z</t>
+  </si>
+  <si>
+    <t>new w_x-&gt;A</t>
+  </si>
+  <si>
+    <t>new w_1-&gt;A</t>
+  </si>
+  <si>
+    <t>new w_2-&gt;A</t>
+  </si>
+  <si>
+    <t>new w_3-&gt;A</t>
+  </si>
+  <si>
+    <t>new w_4-&gt;A</t>
+  </si>
+  <si>
+    <t>new w_x-&gt;B</t>
+  </si>
+  <si>
+    <t>new w_1-&gt;B</t>
+  </si>
+  <si>
+    <t>new w_2-&gt;B</t>
+  </si>
+  <si>
+    <t>new w_3-&gt;B</t>
+  </si>
+  <si>
+    <t>new w_4-&gt;B</t>
+  </si>
+  <si>
+    <t>-------------&gt;</t>
+  </si>
+  <si>
+    <t>&lt;-- NEW PREDICTED OUTCOME</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -336,8 +409,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +478,28 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -505,68 +607,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="12" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="9" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="11" builtinId="41"/>
     <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Accent6" xfId="7" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,43 +997,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E81D6DC-F462-584B-94C4-8AECFCC18FE7}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="14" max="14" width="3.375" customWidth="1"/>
+    <col min="17" max="17" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="12"/>
     </row>
-    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +1045,7 @@
       </c>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -941,7 +1057,7 @@
       </c>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -953,7 +1069,7 @@
       </c>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -965,7 +1081,7 @@
       </c>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -977,7 +1093,7 @@
       </c>
       <c r="N9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1105,7 @@
       </c>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1117,7 @@
       </c>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1129,7 @@
       </c>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1141,7 @@
       </c>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1153,7 @@
       </c>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1165,7 @@
       </c>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1061,7 +1177,7 @@
       </c>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1073,7 +1189,7 @@
       </c>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -1085,13 +1201,13 @@
       </c>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1107,12 +1223,12 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1248,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>1</v>
       </c>
@@ -1149,7 +1265,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>21</v>
       </c>
@@ -1187,7 +1303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="15">
         <v>0.5</v>
       </c>
@@ -1219,152 +1335,611 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="16" cm="1">
-        <f t="array" ref="B31">(1 + EXP(-SUM(B26:F26*B29:F29)))^(-1)</f>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="23" cm="1">
+        <f t="array" ref="B31">SUM(B26:F26*B29:F29)</f>
+        <v>1.7599999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="23" cm="1">
+        <f t="array" ref="B32">SUM(B26:F26*I29:M29)</f>
+        <v>1.9400000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="16">
+        <f>(1 + EXP(-B31))^(-1)</f>
         <v>0.85320966019861766</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="16" cm="1">
-        <f t="array" ref="B32">(1 + EXP(-SUM(B26:F26*I29:M29)))^(-1)</f>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="16">
+        <f>(1 + EXP(-B32))^(-1)</f>
         <v>0.8743521434846544</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B36" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
         <v>0.5</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C37" s="15">
         <v>0.9</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D37" s="15">
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="16">
-        <f xml:space="preserve"> (1 + EXP(-(B26*B35 + B31*C35 + B32*D35)))^(-1)</f>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="23">
+        <f>B26*B37 + B33*C37 + B34*D37</f>
+        <v>2.054805623314945</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="16">
+        <f xml:space="preserve"> (1 + EXP(-(B39)))^(-1)</f>
         <v>0.88643230033488507</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C40" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="21"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="20" t="s">
+      <c r="B47" s="21">
+        <f>-(1-B39)*(B39)*(B26)</f>
+        <v>2.1674205262917745</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="21">
+        <f>$B$37-$D$63*B47</f>
+        <v>8.3855258951979261E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
+      <c r="B48" s="21">
+        <f>-(1-B39)*(B39)*(B33)</f>
+        <v>1.849264130744914</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="21">
+        <f>$C$37-$D$63*B48</f>
+        <v>0.54494128689697652</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="21"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
+      <c r="B49" s="21">
+        <f>-(1-B39)*(B39)*(B34)</f>
+        <v>1.8950887829958507</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="21">
+        <f>$D$37-$D$63*B49</f>
+        <v>0.5361429536647967</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
+      <c r="B51" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$31)*($B$31)*$B$26</f>
+        <v>-2.8991416959678764</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="21">
+        <f>$B$29-$D$63*B51</f>
+        <v>1.0566352056258324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="B52" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$31)*($B$31)*$C$26</f>
+        <v>-1.1596566783871507</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" s="21">
+        <f>$C$29-$D$63*B52</f>
+        <v>0.82265408225033299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="20" t="s">
+      <c r="B53" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$31)*($B$31)*$D$26</f>
+        <v>-2.0293991871775132</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="21">
+        <f>$D$29-$D$63*B53</f>
+        <v>1.1896446439380826</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="21"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
+      <c r="B54" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$31)*($B$31)*$E$26</f>
+        <v>-2.0293991871775132</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="21">
+        <f>$E$29-$D$63*B54</f>
+        <v>0.9896446439380826</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="21"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="20" t="s">
+      <c r="B55" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$31)*($B$31)*$F$26</f>
+        <v>-0.57982833919357535</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F55" s="21">
+        <f>$F$29-$D$63*B55</f>
+        <v>0.31132704112516651</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="21"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="20" t="s">
+      <c r="B57" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$32)*($B$32)*$B$26</f>
+        <v>-3.9525080717456813</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="21">
+        <f>$I$29-$D$63*B57</f>
+        <v>1.4588815497751708</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="21"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
+      <c r="B58" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$32)*($B$32)*$C$26</f>
+        <v>-1.5810032286982727</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="21">
+        <f>$J$29-$D$63*B58</f>
+        <v>1.2035526199100683</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="21"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="20" t="s">
+      <c r="B59" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$32)*($B$32)*$D$26</f>
+        <v>-2.7667556502219766</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="21">
+        <f>$K$29-$D$63*B59</f>
+        <v>1.3312170848426197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="21"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
+      <c r="B60" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$32)*($B$32)*$E$26</f>
+        <v>-2.7667556502219766</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="21">
+        <f>$L$29-$D$63*B60</f>
+        <v>0.93121708484261956</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="21"/>
+      <c r="B61" s="21">
+        <f>-(1-$B$39)*($B$39)*(1-$B$32)*($B$32)*$F$26</f>
+        <v>-0.79050161434913635</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="21">
+        <f>$M$29-$D$63*B61</f>
+        <v>0.35177630995503417</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" s="25">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B67" s="14">
+        <v>1</v>
+      </c>
+      <c r="C67" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D67" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E67" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="F67" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J69" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L69" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M69" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="15">
+        <f>F51</f>
+        <v>1.0566352056258324</v>
+      </c>
+      <c r="C70" s="15">
+        <f>F52</f>
+        <v>0.82265408225033299</v>
+      </c>
+      <c r="D70" s="15">
+        <f>F53</f>
+        <v>1.1896446439380826</v>
+      </c>
+      <c r="E70" s="15">
+        <f>F54</f>
+        <v>0.9896446439380826</v>
+      </c>
+      <c r="F70" s="15">
+        <f>F55</f>
+        <v>0.31132704112516651</v>
+      </c>
+      <c r="I70" s="15">
+        <f>F57</f>
+        <v>1.4588815497751708</v>
+      </c>
+      <c r="J70" s="15">
+        <f>F58</f>
+        <v>1.2035526199100683</v>
+      </c>
+      <c r="K70" s="15">
+        <f>F59</f>
+        <v>1.3312170848426197</v>
+      </c>
+      <c r="L70" s="15">
+        <f>F60</f>
+        <v>0.93121708484261956</v>
+      </c>
+      <c r="M70" s="15">
+        <f>F61</f>
+        <v>0.35177630995503417</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B72" s="23" cm="1">
+        <f t="array" ref="B72">SUM(B67:F67*B70:F70)</f>
+        <v>2.9734647482643144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B73" s="23" cm="1">
+        <f t="array" ref="B73">SUM(B67:F67*I70:M70)</f>
+        <v>3.5943617785098723</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" s="16">
+        <f>(1 + EXP(-B72))^(-1)</f>
+        <v>0.95136085357107703</v>
+      </c>
+      <c r="C74" s="11"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" s="16">
+        <f>(1 + EXP(-B73))^(-1)</f>
+        <v>0.97325664488732799</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="15">
+        <f>F47</f>
+        <v>8.3855258951979261E-2</v>
+      </c>
+      <c r="C78" s="15">
+        <f>F48</f>
+        <v>0.54494128689697652</v>
+      </c>
+      <c r="D78" s="15">
+        <f>F49</f>
+        <v>0.5361429536647967</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="23">
+        <f>B67*B78 + B74*C78 + B75*D78</f>
+        <v>1.1240957590641902</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="16">
+        <f xml:space="preserve"> (1 + EXP(-(B80)))^(-1)</f>
+        <v>0.75474764714099241</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>